<commit_message>
fix (remove) mapping for total C and H industries
</commit_message>
<xml_diff>
--- a/source-data/mappings/euklems-industries-to-fingreen-industries-map.xlsx
+++ b/source-data/mappings/euklems-industries-to-fingreen-industries-map.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="193">
   <si>
     <t xml:space="preserve">nace_r2_code</t>
   </si>
@@ -692,7 +692,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -706,10 +706,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -923,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -932,7 +928,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -946,7 +942,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -998,12 +994,6 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -1075,7 +1065,7 @@
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1094,7 +1084,7 @@
       <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1108,7 +1098,7 @@
       <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1289,12 +1279,6 @@
       <c r="A36" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -1435,7 +1419,7 @@
       <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1446,7 +1430,7 @@
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1542,7 +1526,7 @@
       <c r="C65" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1550,13 +1534,13 @@
       <c r="A66" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1570,7 +1554,7 @@
       <c r="C67" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2119,322 +2103,322 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>